<commit_message>
v0.36.6: Examcell controller and route updated.
</commit_message>
<xml_diff>
--- a/data/template_tg.xlsx
+++ b/data/template_tg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Projects\Web Projects\IntelliCampus\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A999BCC-D541-40DF-B577-6714A36501C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51918184-9A9D-4E96-A994-DE9B88BA0A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D8386E46-D4A0-47E4-93AC-6732B371D031}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9420" xr2:uid="{D8386E46-D4A0-47E4-93AC-6732B371D031}"/>
   </bookViews>
   <sheets>
     <sheet name="Ward_List" sheetId="1" r:id="rId1"/>
@@ -398,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6150553D-B842-4E88-A848-BB8A31A27113}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -417,46 +417,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>202000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>202000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>202000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>202000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>202000004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>202000005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>202000006</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>202000007</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>